<commit_message>
Update 23190_titulos de merced.xlsx
</commit_message>
<xml_diff>
--- a/Pueblos Indígenas/CONADI/23190_titulos de merced.xlsx
+++ b/Pueblos Indígenas/CONADI/23190_titulos de merced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\Diseño DATA's\Tablas Madre\Pueblos Indígenas\CONADI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E01D1B-FA19-4601-B787-49A5D60E7B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E444C8-EC8C-45E8-99C8-B142FEC5C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12050" uniqueCount="6053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12050" uniqueCount="6039">
   <si>
     <t>Título</t>
   </si>
@@ -18147,48 +18147,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>CURACAUTÍN</t>
-  </si>
-  <si>
-    <t>VILCÚN</t>
-  </si>
-  <si>
-    <t>TIRÚA</t>
-  </si>
-  <si>
-    <t>MULCHÉN</t>
-  </si>
-  <si>
-    <t>PITRUFQUÉN</t>
-  </si>
-  <si>
-    <t>PURÉN</t>
-  </si>
-  <si>
-    <t>TOLTÉN</t>
-  </si>
-  <si>
-    <t>TRAIGUÉN</t>
-  </si>
-  <si>
-    <t>PUCÓN</t>
-  </si>
-  <si>
-    <t>CAÑETE</t>
-  </si>
-  <si>
-    <t>RÍO BUENO</t>
-  </si>
-  <si>
-    <t>MÁFIL</t>
-  </si>
-  <si>
-    <t>LA UNIÓN</t>
-  </si>
-  <si>
-    <t>SANTA BÁRBARA</t>
   </si>
   <si>
     <t/>
@@ -18818,12 +18776,29 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right/>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -18834,10 +18809,12 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
         <right/>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -18862,25 +18839,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -18973,10 +18931,10 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Comuna" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Título" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Lugar" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Superficie" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Lugar" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Superficie" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Año" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Descripción" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Descripción" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Codcom"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -19306,8 +19264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3011"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2987" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3011"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19340,7 +19298,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>6052</v>
+        <v>6038</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -19391,7 +19349,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6037</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -19426,7 +19384,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -19592,7 +19550,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>42</v>
@@ -19717,7 +19675,7 @@
         <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -19906,7 +19864,7 @@
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>6037</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>90</v>
@@ -19952,7 +19910,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>96</v>
@@ -19998,7 +19956,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>103</v>
@@ -20192,7 +20150,7 @@
         <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -20473,7 +20431,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>6040</v>
+        <v>163</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>160</v>
@@ -20496,7 +20454,7 @@
     </row>
     <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>164</v>
@@ -20565,7 +20523,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>173</v>
@@ -20588,7 +20546,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>176</v>
@@ -20611,7 +20569,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>177</v>
@@ -20634,7 +20592,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>6040</v>
+        <v>163</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>181</v>
@@ -21081,7 +21039,7 @@
         <v>62</v>
       </c>
       <c r="G78" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -21142,7 +21100,7 @@
         <v>62</v>
       </c>
       <c r="G81" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -21515,7 +21473,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>271</v>
@@ -21538,7 +21496,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>274</v>
@@ -21640,7 +21598,7 @@
         <v>62</v>
       </c>
       <c r="G103" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -21816,12 +21774,12 @@
         <v>302</v>
       </c>
       <c r="G111" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>303</v>
@@ -21854,7 +21812,7 @@
         <v>62</v>
       </c>
       <c r="G113" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -21882,7 +21840,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>309</v>
@@ -21905,7 +21863,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>312</v>
@@ -22398,7 +22356,7 @@
         <v>62</v>
       </c>
       <c r="G137" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -22426,7 +22384,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>370</v>
@@ -22472,7 +22430,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>376</v>
@@ -22495,7 +22453,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>378</v>
@@ -22564,7 +22522,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>385</v>
@@ -22587,7 +22545,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>388</v>
@@ -22610,7 +22568,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>391</v>
@@ -22725,7 +22683,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>400</v>
@@ -22909,7 +22867,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>417</v>
@@ -23264,7 +23222,7 @@
         <v>62</v>
       </c>
       <c r="G175" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -23292,7 +23250,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>453</v>
@@ -23315,7 +23273,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>454</v>
@@ -23637,7 +23595,7 @@
     </row>
     <row r="192" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>482</v>
@@ -23660,7 +23618,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>485</v>
@@ -23706,7 +23664,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>491</v>
@@ -23821,7 +23779,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>501</v>
@@ -23844,7 +23802,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>502</v>
@@ -23969,7 +23927,7 @@
         <v>62</v>
       </c>
       <c r="G206" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -24020,7 +23978,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>519</v>
@@ -24053,7 +24011,7 @@
         <v>62</v>
       </c>
       <c r="G210" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -24160,7 +24118,7 @@
         <v>62</v>
       </c>
       <c r="G215" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -24257,7 +24215,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>541</v>
@@ -24579,7 +24537,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>571</v>
@@ -24648,7 +24606,7 @@
     </row>
     <row r="237" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>577</v>
@@ -24704,7 +24662,7 @@
         <v>62</v>
       </c>
       <c r="G239" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="240" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -24824,7 +24782,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>597</v>
@@ -24893,7 +24851,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>604</v>
@@ -24916,7 +24874,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>605</v>
@@ -24939,7 +24897,7 @@
     </row>
     <row r="250" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>606</v>
@@ -25008,7 +24966,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>615</v>
@@ -25031,7 +24989,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>618</v>
@@ -25156,7 +25114,7 @@
         <v>62</v>
       </c>
       <c r="G259" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="260" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -25230,7 +25188,7 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>636</v>
@@ -25263,7 +25221,7 @@
         <v>640</v>
       </c>
       <c r="G264" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -25278,12 +25236,12 @@
         <v>640</v>
       </c>
       <c r="G265" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="266" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>642</v>
@@ -25973,7 +25931,7 @@
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>708</v>
@@ -26008,12 +25966,12 @@
         <v>712</v>
       </c>
       <c r="G297" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="298" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>714</v>
@@ -26036,7 +25994,7 @@
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>717</v>
@@ -26059,7 +26017,7 @@
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>720</v>
@@ -26105,7 +26063,7 @@
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>726</v>
@@ -26128,7 +26086,7 @@
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>728</v>
@@ -26197,7 +26155,7 @@
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>734</v>
@@ -26289,7 +26247,7 @@
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>743</v>
@@ -26450,7 +26408,7 @@
     </row>
     <row r="317" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A317" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>756</v>
@@ -26473,7 +26431,7 @@
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>759</v>
@@ -26565,7 +26523,7 @@
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A322" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>767</v>
@@ -26611,7 +26569,7 @@
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A324" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>771</v>
@@ -26634,7 +26592,7 @@
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>774</v>
@@ -26657,7 +26615,7 @@
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A326" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>777</v>
@@ -26680,7 +26638,7 @@
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A327" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>779</v>
@@ -26736,7 +26694,7 @@
         <v>62</v>
       </c>
       <c r="G329" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.3">
@@ -26751,7 +26709,7 @@
         <v>62</v>
       </c>
       <c r="G330" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.3">
@@ -26766,7 +26724,7 @@
         <v>62</v>
       </c>
       <c r="G331" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.3">
@@ -26781,7 +26739,7 @@
         <v>62</v>
       </c>
       <c r="G332" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.3">
@@ -26901,7 +26859,7 @@
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>798</v>
@@ -28143,7 +28101,7 @@
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A392" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>917</v>
@@ -28373,7 +28331,7 @@
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A402" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B402" s="1" t="s">
         <v>947</v>
@@ -28534,7 +28492,7 @@
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A409" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B409" s="1" t="s">
         <v>968</v>
@@ -28741,7 +28699,7 @@
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A418" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B418" s="1" t="s">
         <v>992</v>
@@ -28948,7 +28906,7 @@
     </row>
     <row r="427" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A427" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B427" s="1" t="s">
         <v>1013</v>
@@ -28994,7 +28952,7 @@
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A429" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B429" s="1" t="s">
         <v>1019</v>
@@ -29178,7 +29136,7 @@
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A437" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B437" s="1" t="s">
         <v>1041</v>
@@ -29201,7 +29159,7 @@
     </row>
     <row r="438" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A438" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B438" s="1" t="s">
         <v>1043</v>
@@ -29224,7 +29182,7 @@
     </row>
     <row r="439" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A439" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>1046</v>
@@ -29247,7 +29205,7 @@
     </row>
     <row r="440" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A440" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>1047</v>
@@ -29431,7 +29389,7 @@
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A448" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B448" s="1" t="s">
         <v>1068</v>
@@ -29454,7 +29412,7 @@
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A449" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B449" s="1" t="s">
         <v>1069</v>
@@ -29500,7 +29458,7 @@
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A451" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B451" s="1" t="s">
         <v>1073</v>
@@ -29523,7 +29481,7 @@
     </row>
     <row r="452" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A452" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B452" s="1" t="s">
         <v>1074</v>
@@ -29546,7 +29504,7 @@
     </row>
     <row r="453" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A453" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B453" s="1" t="s">
         <v>1077</v>
@@ -29569,7 +29527,7 @@
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A454" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B454" s="1" t="s">
         <v>1080</v>
@@ -29615,7 +29573,7 @@
     </row>
     <row r="456" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A456" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B456" s="1" t="s">
         <v>1084</v>
@@ -29822,7 +29780,7 @@
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A465" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B465" s="1" t="s">
         <v>1103</v>
@@ -29891,7 +29849,7 @@
     </row>
     <row r="468" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A468" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B468" s="1" t="s">
         <v>1111</v>
@@ -29937,7 +29895,7 @@
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A470" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B470" s="1" t="s">
         <v>1117</v>
@@ -29960,7 +29918,7 @@
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A471" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B471" s="1" t="s">
         <v>1118</v>
@@ -30029,7 +29987,7 @@
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A474" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B474" s="1" t="s">
         <v>1123</v>
@@ -30558,7 +30516,7 @@
     </row>
     <row r="497" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A497" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B497" s="1" t="s">
         <v>1171</v>
@@ -30788,7 +30746,7 @@
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A507" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B507" s="1" t="s">
         <v>1193</v>
@@ -30903,7 +30861,7 @@
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A512" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B512" s="1" t="s">
         <v>1202</v>
@@ -30995,7 +30953,7 @@
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A516" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B516" s="1" t="s">
         <v>1207</v>
@@ -31041,7 +30999,7 @@
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A518" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B518" s="1" t="s">
         <v>1210</v>
@@ -31087,7 +31045,7 @@
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A520" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B520" s="1" t="s">
         <v>1216</v>
@@ -31202,7 +31160,7 @@
     </row>
     <row r="525" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A525" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B525" s="1" t="s">
         <v>1226</v>
@@ -31248,7 +31206,7 @@
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A527" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B527" s="1" t="s">
         <v>1230</v>
@@ -31271,7 +31229,7 @@
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A528" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B528" s="1" t="s">
         <v>1233</v>
@@ -31294,7 +31252,7 @@
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A529" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B529" s="1" t="s">
         <v>1234</v>
@@ -31317,7 +31275,7 @@
     </row>
     <row r="530" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A530" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B530" s="1" t="s">
         <v>1235</v>
@@ -31363,7 +31321,7 @@
     </row>
     <row r="532" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A532" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B532" s="1" t="s">
         <v>1240</v>
@@ -31386,7 +31344,7 @@
     </row>
     <row r="533" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A533" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B533" s="1" t="s">
         <v>1243</v>
@@ -31409,7 +31367,7 @@
     </row>
     <row r="534" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A534" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B534" s="1" t="s">
         <v>1244</v>
@@ -31467,12 +31425,12 @@
         <v>1249</v>
       </c>
       <c r="G536" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A537" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B537" s="1" t="s">
         <v>1250</v>
@@ -31495,7 +31453,7 @@
     </row>
     <row r="538" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A538" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B538" s="1" t="s">
         <v>1253</v>
@@ -31898,7 +31856,7 @@
         <v>1290</v>
       </c>
       <c r="G555" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.3">
@@ -32030,7 +31988,7 @@
         <v>1290</v>
       </c>
       <c r="G561" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.3">
@@ -32196,7 +32154,7 @@
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A569" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B569" s="1" t="s">
         <v>1313</v>
@@ -32438,7 +32396,7 @@
         <v>1290</v>
       </c>
       <c r="G579" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="580" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -32478,7 +32436,7 @@
         <v>1290</v>
       </c>
       <c r="G581" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="582" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -32575,7 +32533,7 @@
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A586" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B586" s="1" t="s">
         <v>1344</v>
@@ -32851,7 +32809,7 @@
     </row>
     <row r="598" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A598" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B598" s="1" t="s">
         <v>1371</v>
@@ -32874,7 +32832,7 @@
     </row>
     <row r="599" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A599" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B599" s="1" t="s">
         <v>1374</v>
@@ -32920,7 +32878,7 @@
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A601" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B601" s="1" t="s">
         <v>1380</v>
@@ -32966,7 +32924,7 @@
     </row>
     <row r="603" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A603" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B603" s="1" t="s">
         <v>1385</v>
@@ -33012,7 +32970,7 @@
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A605" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B605" s="1" t="s">
         <v>1388</v>
@@ -33081,7 +33039,7 @@
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A608" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B608" s="1" t="s">
         <v>1395</v>
@@ -33288,7 +33246,7 @@
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A617" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B617" s="1" t="s">
         <v>1411</v>
@@ -33357,7 +33315,7 @@
     </row>
     <row r="620" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A620" s="2" t="s">
-        <v>6037</v>
+        <v>16</v>
       </c>
       <c r="B620" s="1" t="s">
         <v>1417</v>
@@ -33507,7 +33465,7 @@
         <v>1428</v>
       </c>
       <c r="G626" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="627" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -33593,7 +33551,7 @@
         <v>1290</v>
       </c>
       <c r="G630" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.3">
@@ -33644,7 +33602,7 @@
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A633" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B633" s="1" t="s">
         <v>1440</v>
@@ -33759,7 +33717,7 @@
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A638" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B638" s="1" t="s">
         <v>1452</v>
@@ -33851,7 +33809,7 @@
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A642" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B642" s="1" t="s">
         <v>1462</v>
@@ -33874,7 +33832,7 @@
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B643" s="1" t="s">
         <v>1465</v>
@@ -33897,7 +33855,7 @@
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A644" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B644" s="1" t="s">
         <v>1468</v>
@@ -33955,7 +33913,7 @@
         <v>1473</v>
       </c>
       <c r="G646" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="647" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -34006,7 +33964,7 @@
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A649" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B649" s="1" t="s">
         <v>1476</v>
@@ -34098,7 +34056,7 @@
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B653" s="1" t="s">
         <v>1484</v>
@@ -34167,7 +34125,7 @@
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B656" s="1" t="s">
         <v>1490</v>
@@ -34213,7 +34171,7 @@
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B658" s="1" t="s">
         <v>1495</v>
@@ -34248,7 +34206,7 @@
         <v>1497</v>
       </c>
       <c r="G659" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.3">
@@ -34414,7 +34372,7 @@
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B667" s="1" t="s">
         <v>1508</v>
@@ -34506,7 +34464,7 @@
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A671" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B671" s="1" t="s">
         <v>1516</v>
@@ -34529,7 +34487,7 @@
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A672" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B672" s="1" t="s">
         <v>1517</v>
@@ -34713,7 +34671,7 @@
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B680" s="1" t="s">
         <v>1528</v>
@@ -34759,7 +34717,7 @@
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B682" s="1" t="s">
         <v>1532</v>
@@ -34874,7 +34832,7 @@
     </row>
     <row r="687" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B687" s="1" t="s">
         <v>1546</v>
@@ -34897,7 +34855,7 @@
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B688" s="1" t="s">
         <v>1549</v>
@@ -34920,7 +34878,7 @@
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B689" s="1" t="s">
         <v>1552</v>
@@ -34943,7 +34901,7 @@
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B690" s="1" t="s">
         <v>1555</v>
@@ -35012,7 +34970,7 @@
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B693" s="1" t="s">
         <v>1562</v>
@@ -35058,7 +35016,7 @@
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B695" s="1" t="s">
         <v>1567</v>
@@ -35104,7 +35062,7 @@
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A697" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B697" s="1" t="s">
         <v>1572</v>
@@ -35127,7 +35085,7 @@
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A698" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B698" s="1" t="s">
         <v>1573</v>
@@ -35288,7 +35246,7 @@
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B705" s="1" t="s">
         <v>1586</v>
@@ -35334,7 +35292,7 @@
     </row>
     <row r="707" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B707" s="1" t="s">
         <v>1590</v>
@@ -35357,7 +35315,7 @@
     </row>
     <row r="708" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B708" s="1" t="s">
         <v>1592</v>
@@ -35426,7 +35384,7 @@
     </row>
     <row r="711" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B711" s="1" t="s">
         <v>1599</v>
@@ -35495,7 +35453,7 @@
     </row>
     <row r="714" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A714" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B714" s="1" t="s">
         <v>1607</v>
@@ -35518,7 +35476,7 @@
     </row>
     <row r="715" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B715" s="1" t="s">
         <v>1610</v>
@@ -35610,7 +35568,7 @@
     </row>
     <row r="719" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B719" s="1" t="s">
         <v>1618</v>
@@ -35633,7 +35591,7 @@
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B720" s="1" t="s">
         <v>1620</v>
@@ -35656,7 +35614,7 @@
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B721" s="1" t="s">
         <v>1621</v>
@@ -35679,7 +35637,7 @@
     </row>
     <row r="722" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B722" s="1" t="s">
         <v>1622</v>
@@ -35702,7 +35660,7 @@
     </row>
     <row r="723" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B723" s="1" t="s">
         <v>1625</v>
@@ -35725,7 +35683,7 @@
     </row>
     <row r="724" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B724" s="1" t="s">
         <v>1626</v>
@@ -35748,7 +35706,7 @@
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B725" s="1" t="s">
         <v>1627</v>
@@ -35771,7 +35729,7 @@
     </row>
     <row r="726" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B726" s="1" t="s">
         <v>1628</v>
@@ -35840,7 +35798,7 @@
     </row>
     <row r="729" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B729" s="1" t="s">
         <v>1633</v>
@@ -36024,7 +35982,7 @@
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B737" s="1" t="s">
         <v>1651</v>
@@ -36254,7 +36212,7 @@
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B747" s="1" t="s">
         <v>1668</v>
@@ -36576,7 +36534,7 @@
     </row>
     <row r="761" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A761" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B761" s="1" t="s">
         <v>1700</v>
@@ -36599,7 +36557,7 @@
     </row>
     <row r="762" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A762" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B762" s="1" t="s">
         <v>1701</v>
@@ -36622,7 +36580,7 @@
     </row>
     <row r="763" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A763" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B763" s="1" t="s">
         <v>1704</v>
@@ -36645,7 +36603,7 @@
     </row>
     <row r="764" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A764" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B764" s="1" t="s">
         <v>1705</v>
@@ -37059,7 +37017,7 @@
     </row>
     <row r="782" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A782" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B782" s="1" t="s">
         <v>1746</v>
@@ -37358,7 +37316,7 @@
     </row>
     <row r="795" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A795" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B795" s="1" t="s">
         <v>1775</v>
@@ -38002,7 +37960,7 @@
     </row>
     <row r="823" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A823" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B823" s="1" t="s">
         <v>1815</v>
@@ -38416,7 +38374,7 @@
     </row>
     <row r="841" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A841" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B841" s="1" t="s">
         <v>1840</v>
@@ -38439,7 +38397,7 @@
     </row>
     <row r="842" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A842" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B842" s="1" t="s">
         <v>1842</v>
@@ -38508,7 +38466,7 @@
     </row>
     <row r="845" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A845" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B845" s="1" t="s">
         <v>1845</v>
@@ -38577,7 +38535,7 @@
     </row>
     <row r="848" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A848" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B848" s="1" t="s">
         <v>1851</v>
@@ -38771,12 +38729,12 @@
         <v>62</v>
       </c>
       <c r="G856" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A857" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>1876</v>
@@ -38799,7 +38757,7 @@
     </row>
     <row r="858" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A858" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B858" s="1" t="s">
         <v>1878</v>
@@ -39246,12 +39204,12 @@
         <v>62</v>
       </c>
       <c r="G877" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="878" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A878" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B878" s="1" t="s">
         <v>1926</v>
@@ -39274,7 +39232,7 @@
     </row>
     <row r="879" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A879" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B879" s="1" t="s">
         <v>1930</v>
@@ -39297,7 +39255,7 @@
     </row>
     <row r="880" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A880" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B880" s="1" t="s">
         <v>1933</v>
@@ -39905,12 +39863,12 @@
         <v>640</v>
       </c>
       <c r="G906" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="907" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A907" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B907" s="1" t="s">
         <v>1986</v>
@@ -40355,7 +40313,7 @@
         <v>2025</v>
       </c>
       <c r="G926" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="927" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -41027,7 +40985,7 @@
     </row>
     <row r="956" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A956" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B956" s="1" t="s">
         <v>2084</v>
@@ -41487,7 +41445,7 @@
     </row>
     <row r="976" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A976" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B976" s="1" t="s">
         <v>2131</v>
@@ -41648,7 +41606,7 @@
     </row>
     <row r="983" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A983" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B983" s="1" t="s">
         <v>2145</v>
@@ -41993,7 +41951,7 @@
     </row>
     <row r="998" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A998" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B998" s="1" t="s">
         <v>2174</v>
@@ -42085,7 +42043,7 @@
     </row>
     <row r="1002" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1002" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1002" s="1" t="s">
         <v>2182</v>
@@ -42189,7 +42147,7 @@
         <v>2192</v>
       </c>
       <c r="G1006" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1007" spans="1:7" x14ac:dyDescent="0.3">
@@ -42434,7 +42392,7 @@
         <v>640</v>
       </c>
       <c r="G1017" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1018" spans="1:7" x14ac:dyDescent="0.3">
@@ -42468,7 +42426,7 @@
         <v>2220</v>
       </c>
       <c r="G1019" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1020" spans="1:7" x14ac:dyDescent="0.3">
@@ -42519,7 +42477,7 @@
     </row>
     <row r="1022" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1022" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1022" s="1" t="s">
         <v>2227</v>
@@ -42588,7 +42546,7 @@
     </row>
     <row r="1025" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1025" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1025" s="1" t="s">
         <v>2235</v>
@@ -42713,7 +42671,7 @@
         <v>640</v>
       </c>
       <c r="G1030" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1031" spans="1:7" x14ac:dyDescent="0.3">
@@ -42994,7 +42952,7 @@
     </row>
     <row r="1043" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1043" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1043" s="1" t="s">
         <v>2266</v>
@@ -44282,7 +44240,7 @@
     </row>
     <row r="1099" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1099" s="2" t="s">
-        <v>6040</v>
+        <v>163</v>
       </c>
       <c r="B1099" s="1" t="s">
         <v>2370</v>
@@ -44568,7 +44526,7 @@
         <v>62</v>
       </c>
       <c r="G1111" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1112" spans="1:7" x14ac:dyDescent="0.3">
@@ -44619,7 +44577,7 @@
     </row>
     <row r="1114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1114" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B1114" s="1" t="s">
         <v>2402</v>
@@ -44987,7 +44945,7 @@
     </row>
     <row r="1130" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1130" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B1130" s="1" t="s">
         <v>2436</v>
@@ -45528,12 +45486,12 @@
         <v>2493</v>
       </c>
       <c r="G1153" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1154" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1154" s="1" t="s">
         <v>2495</v>
@@ -45556,7 +45514,7 @@
     </row>
     <row r="1155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1155" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1155" s="1" t="s">
         <v>2496</v>
@@ -45579,7 +45537,7 @@
     </row>
     <row r="1156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1156" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1156" s="1" t="s">
         <v>2499</v>
@@ -45773,7 +45731,7 @@
         <v>640</v>
       </c>
       <c r="G1164" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1165" spans="1:7" x14ac:dyDescent="0.3">
@@ -45939,7 +45897,7 @@
     </row>
     <row r="1172" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1172" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1172" s="1" t="s">
         <v>2534</v>
@@ -46020,7 +45978,7 @@
         <v>2541</v>
       </c>
       <c r="G1175" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1176" spans="1:7" x14ac:dyDescent="0.3">
@@ -46140,7 +46098,7 @@
     </row>
     <row r="1181" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1181" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1181" s="1" t="s">
         <v>2552</v>
@@ -46209,7 +46167,7 @@
     </row>
     <row r="1184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1184" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1184" s="1" t="s">
         <v>2558</v>
@@ -46232,7 +46190,7 @@
     </row>
     <row r="1185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1185" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1185" s="1" t="s">
         <v>2562</v>
@@ -46265,7 +46223,7 @@
         <v>640</v>
       </c>
       <c r="G1186" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1187" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -46293,7 +46251,7 @@
     </row>
     <row r="1188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1188" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1188" s="1" t="s">
         <v>2569</v>
@@ -46316,7 +46274,7 @@
     </row>
     <row r="1189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1189" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1189" s="1" t="s">
         <v>2570</v>
@@ -46385,7 +46343,7 @@
     </row>
     <row r="1192" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1192" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1192" s="1" t="s">
         <v>2575</v>
@@ -46408,7 +46366,7 @@
     </row>
     <row r="1193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1193" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1193" s="1" t="s">
         <v>2578</v>
@@ -46431,7 +46389,7 @@
     </row>
     <row r="1194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1194" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1194" s="1" t="s">
         <v>2581</v>
@@ -46454,7 +46412,7 @@
     </row>
     <row r="1195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1195" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1195" s="1" t="s">
         <v>2584</v>
@@ -46477,7 +46435,7 @@
     </row>
     <row r="1196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1196" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1196" s="1" t="s">
         <v>2587</v>
@@ -46523,7 +46481,7 @@
     </row>
     <row r="1198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1198" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1198" s="1" t="s">
         <v>2592</v>
@@ -46546,7 +46504,7 @@
     </row>
     <row r="1199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1199" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1199" s="1" t="s">
         <v>2595</v>
@@ -46569,7 +46527,7 @@
     </row>
     <row r="1200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1200" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1200" s="1" t="s">
         <v>2596</v>
@@ -46592,7 +46550,7 @@
     </row>
     <row r="1201" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1201" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1201" s="1" t="s">
         <v>2597</v>
@@ -46638,7 +46596,7 @@
     </row>
     <row r="1203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1203" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1203" s="1" t="s">
         <v>2599</v>
@@ -46763,7 +46721,7 @@
         <v>2612</v>
       </c>
       <c r="G1208" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1209" spans="1:7" x14ac:dyDescent="0.3">
@@ -47008,7 +46966,7 @@
         <v>62</v>
       </c>
       <c r="G1219" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1220" spans="1:7" x14ac:dyDescent="0.3">
@@ -47289,7 +47247,7 @@
     </row>
     <row r="1232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1232" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1232" s="1" t="s">
         <v>2661</v>
@@ -47404,7 +47362,7 @@
     </row>
     <row r="1237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1237" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1237" s="1" t="s">
         <v>2673</v>
@@ -47552,7 +47510,7 @@
         <v>671</v>
       </c>
       <c r="G1243" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1244" spans="1:7" x14ac:dyDescent="0.3">
@@ -48201,7 +48159,7 @@
     </row>
     <row r="1272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1272" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1272" s="1" t="s">
         <v>2740</v>
@@ -48477,7 +48435,7 @@
     </row>
     <row r="1284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1284" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1284" s="1" t="s">
         <v>2764</v>
@@ -48638,7 +48596,7 @@
     </row>
     <row r="1291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1291" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1291" s="1" t="s">
         <v>2777</v>
@@ -48661,7 +48619,7 @@
     </row>
     <row r="1292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1292" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1292" s="1" t="s">
         <v>2778</v>
@@ -48776,7 +48734,7 @@
     </row>
     <row r="1297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1297" s="2" t="s">
-        <v>6048</v>
+        <v>2791</v>
       </c>
       <c r="B1297" s="1" t="s">
         <v>2788</v>
@@ -48868,7 +48826,7 @@
     </row>
     <row r="1301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1301" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B1301" s="1" t="s">
         <v>2798</v>
@@ -48914,7 +48872,7 @@
     </row>
     <row r="1303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1303" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1303" s="1" t="s">
         <v>2802</v>
@@ -49374,7 +49332,7 @@
     </row>
     <row r="1323" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1323" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B1323" s="1" t="s">
         <v>2837</v>
@@ -49420,7 +49378,7 @@
     </row>
     <row r="1325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1325" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1325" s="1" t="s">
         <v>2841</v>
@@ -49535,7 +49493,7 @@
     </row>
     <row r="1330" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1330" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1330" s="1" t="s">
         <v>2852</v>
@@ -49558,7 +49516,7 @@
     </row>
     <row r="1331" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1331" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1331" s="1" t="s">
         <v>2854</v>
@@ -49581,7 +49539,7 @@
     </row>
     <row r="1332" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1332" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1332" s="1" t="s">
         <v>2856</v>
@@ -49627,7 +49585,7 @@
     </row>
     <row r="1334" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1334" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1334" s="1" t="s">
         <v>2860</v>
@@ -50139,7 +50097,7 @@
         <v>915</v>
       </c>
       <c r="G1356" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1357" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -50213,7 +50171,7 @@
     </row>
     <row r="1360" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1360" s="2" t="s">
-        <v>6048</v>
+        <v>2791</v>
       </c>
       <c r="B1360" s="1" t="s">
         <v>2908</v>
@@ -50512,7 +50470,7 @@
     </row>
     <row r="1373" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1373" s="2" t="s">
-        <v>6048</v>
+        <v>2791</v>
       </c>
       <c r="B1373" s="1" t="s">
         <v>2937</v>
@@ -50719,7 +50677,7 @@
     </row>
     <row r="1382" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1382" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1382" s="1" t="s">
         <v>2951</v>
@@ -50742,7 +50700,7 @@
     </row>
     <row r="1383" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1383" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1383" s="1" t="s">
         <v>2953</v>
@@ -50765,7 +50723,7 @@
     </row>
     <row r="1384" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1384" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1384" s="1" t="s">
         <v>2954</v>
@@ -50788,7 +50746,7 @@
     </row>
     <row r="1385" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1385" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1385" s="1" t="s">
         <v>2957</v>
@@ -50811,7 +50769,7 @@
     </row>
     <row r="1386" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1386" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1386" s="1" t="s">
         <v>2960</v>
@@ -50857,7 +50815,7 @@
     </row>
     <row r="1388" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1388" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1388" s="1" t="s">
         <v>2965</v>
@@ -50880,7 +50838,7 @@
     </row>
     <row r="1389" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1389" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1389" s="1" t="s">
         <v>2966</v>
@@ -50926,7 +50884,7 @@
     </row>
     <row r="1391" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1391" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1391" s="1" t="s">
         <v>2970</v>
@@ -50972,7 +50930,7 @@
     </row>
     <row r="1393" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1393" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1393" s="1" t="s">
         <v>2974</v>
@@ -50995,7 +50953,7 @@
     </row>
     <row r="1394" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1394" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1394" s="1" t="s">
         <v>2976</v>
@@ -51018,7 +50976,7 @@
     </row>
     <row r="1395" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1395" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1395" s="1" t="s">
         <v>2979</v>
@@ -51041,7 +50999,7 @@
     </row>
     <row r="1396" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1396" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1396" s="1" t="s">
         <v>2982</v>
@@ -51064,7 +51022,7 @@
     </row>
     <row r="1397" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1397" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1397" s="1" t="s">
         <v>2985</v>
@@ -51202,7 +51160,7 @@
     </row>
     <row r="1403" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1403" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1403" s="1" t="s">
         <v>2995</v>
@@ -51225,7 +51183,7 @@
     </row>
     <row r="1404" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1404" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1404" s="1" t="s">
         <v>2998</v>
@@ -51294,7 +51252,7 @@
     </row>
     <row r="1407" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1407" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1407" s="1" t="s">
         <v>3005</v>
@@ -51317,7 +51275,7 @@
     </row>
     <row r="1408" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1408" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1408" s="1" t="s">
         <v>3008</v>
@@ -51731,7 +51689,7 @@
     </row>
     <row r="1426" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1426" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B1426" s="1" t="s">
         <v>3032</v>
@@ -52076,7 +52034,7 @@
     </row>
     <row r="1441" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1441" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1441" s="1" t="s">
         <v>3057</v>
@@ -52467,7 +52425,7 @@
     </row>
     <row r="1458" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1458" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1458" s="1" t="s">
         <v>3085</v>
@@ -52490,7 +52448,7 @@
     </row>
     <row r="1459" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1459" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1459" s="1" t="s">
         <v>3088</v>
@@ -52513,7 +52471,7 @@
     </row>
     <row r="1460" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1460" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1460" s="1" t="s">
         <v>3089</v>
@@ -52536,7 +52494,7 @@
     </row>
     <row r="1461" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1461" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1461" s="1" t="s">
         <v>3090</v>
@@ -52628,7 +52586,7 @@
     </row>
     <row r="1465" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1465" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1465" s="1" t="s">
         <v>3098</v>
@@ -52720,7 +52678,7 @@
     </row>
     <row r="1469" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1469" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1469" s="1" t="s">
         <v>3105</v>
@@ -52743,7 +52701,7 @@
     </row>
     <row r="1470" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1470" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1470" s="1" t="s">
         <v>3106</v>
@@ -52766,7 +52724,7 @@
     </row>
     <row r="1471" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1471" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1471" s="1" t="s">
         <v>3107</v>
@@ -52789,7 +52747,7 @@
     </row>
     <row r="1472" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1472" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1472" s="1" t="s">
         <v>3108</v>
@@ -52812,7 +52770,7 @@
     </row>
     <row r="1473" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1473" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1473" s="1" t="s">
         <v>3109</v>
@@ -52835,7 +52793,7 @@
     </row>
     <row r="1474" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1474" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1474" s="1" t="s">
         <v>3112</v>
@@ -52858,7 +52816,7 @@
     </row>
     <row r="1475" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1475" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1475" s="1" t="s">
         <v>3115</v>
@@ -52881,7 +52839,7 @@
     </row>
     <row r="1476" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1476" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1476" s="1" t="s">
         <v>3117</v>
@@ -52904,7 +52862,7 @@
     </row>
     <row r="1477" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1477" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1477" s="1" t="s">
         <v>3118</v>
@@ -52927,7 +52885,7 @@
     </row>
     <row r="1478" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1478" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1478" s="1" t="s">
         <v>3119</v>
@@ -52996,7 +52954,7 @@
     </row>
     <row r="1481" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1481" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1481" s="1" t="s">
         <v>3124</v>
@@ -53065,7 +53023,7 @@
     </row>
     <row r="1484" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1484" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1484" s="1" t="s">
         <v>3131</v>
@@ -53111,7 +53069,7 @@
     </row>
     <row r="1486" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1486" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1486" s="1" t="s">
         <v>3133</v>
@@ -53226,7 +53184,7 @@
     </row>
     <row r="1491" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1491" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B1491" s="1" t="s">
         <v>3143</v>
@@ -53341,7 +53299,7 @@
     </row>
     <row r="1496" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1496" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1496" s="1" t="s">
         <v>3152</v>
@@ -53797,7 +53755,7 @@
     </row>
     <row r="1516" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1516" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1516" s="1" t="s">
         <v>3196</v>
@@ -56224,7 +56182,7 @@
         <v>3405</v>
       </c>
       <c r="G1621" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1622" spans="1:7" x14ac:dyDescent="0.3">
@@ -56689,7 +56647,7 @@
     </row>
     <row r="1642" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1642" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1642" s="1" t="s">
         <v>3450</v>
@@ -56735,7 +56693,7 @@
     </row>
     <row r="1644" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1644" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B1644" s="1" t="s">
         <v>3454</v>
@@ -56850,7 +56808,7 @@
     </row>
     <row r="1649" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1649" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B1649" s="1" t="s">
         <v>3466</v>
@@ -56896,7 +56854,7 @@
     </row>
     <row r="1651" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1651" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1651" s="1" t="s">
         <v>3470</v>
@@ -56919,7 +56877,7 @@
     </row>
     <row r="1652" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1652" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1652" s="1" t="s">
         <v>3471</v>
@@ -56942,7 +56900,7 @@
     </row>
     <row r="1653" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1653" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1653" s="1" t="s">
         <v>3473</v>
@@ -56965,7 +56923,7 @@
     </row>
     <row r="1654" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1654" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1654" s="1" t="s">
         <v>3475</v>
@@ -56988,7 +56946,7 @@
     </row>
     <row r="1655" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1655" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1655" s="1" t="s">
         <v>3476</v>
@@ -57011,7 +56969,7 @@
     </row>
     <row r="1656" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1656" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1656" s="1" t="s">
         <v>3477</v>
@@ -57057,7 +57015,7 @@
     </row>
     <row r="1658" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1658" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1658" s="1" t="s">
         <v>3479</v>
@@ -57080,7 +57038,7 @@
     </row>
     <row r="1659" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1659" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1659" s="1" t="s">
         <v>3480</v>
@@ -57103,7 +57061,7 @@
     </row>
     <row r="1660" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1660" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1660" s="1" t="s">
         <v>3481</v>
@@ -57172,7 +57130,7 @@
     </row>
     <row r="1663" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1663" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1663" s="1" t="s">
         <v>3488</v>
@@ -57264,7 +57222,7 @@
     </row>
     <row r="1667" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1667" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1667" s="1" t="s">
         <v>3493</v>
@@ -57310,7 +57268,7 @@
     </row>
     <row r="1669" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1669" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1669" s="1" t="s">
         <v>3495</v>
@@ -57333,7 +57291,7 @@
     </row>
     <row r="1670" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1670" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1670" s="1" t="s">
         <v>3498</v>
@@ -57356,7 +57314,7 @@
     </row>
     <row r="1671" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1671" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1671" s="1" t="s">
         <v>3501</v>
@@ -57425,7 +57383,7 @@
     </row>
     <row r="1674" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1674" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1674" s="1" t="s">
         <v>3505</v>
@@ -57609,7 +57567,7 @@
     </row>
     <row r="1682" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1682" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1682" s="1" t="s">
         <v>3518</v>
@@ -57632,7 +57590,7 @@
     </row>
     <row r="1683" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1683" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B1683" s="1" t="s">
         <v>3520</v>
@@ -57655,7 +57613,7 @@
     </row>
     <row r="1684" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1684" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1684" s="1" t="s">
         <v>3521</v>
@@ -57701,7 +57659,7 @@
     </row>
     <row r="1686" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1686" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B1686" s="1" t="s">
         <v>3523</v>
@@ -57747,7 +57705,7 @@
     </row>
     <row r="1688" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1688" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1688" s="1" t="s">
         <v>3527</v>
@@ -57770,7 +57728,7 @@
     </row>
     <row r="1689" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1689" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1689" s="1" t="s">
         <v>3530</v>
@@ -58092,7 +58050,7 @@
     </row>
     <row r="1703" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1703" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1703" s="1" t="s">
         <v>3560</v>
@@ -58115,7 +58073,7 @@
     </row>
     <row r="1704" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1704" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1704" s="1" t="s">
         <v>3562</v>
@@ -58138,7 +58096,7 @@
     </row>
     <row r="1705" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1705" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1705" s="1" t="s">
         <v>3563</v>
@@ -58345,7 +58303,7 @@
     </row>
     <row r="1714" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1714" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1714" s="1" t="s">
         <v>3576</v>
@@ -59265,7 +59223,7 @@
     </row>
     <row r="1754" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1754" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1754" s="1" t="s">
         <v>3658</v>
@@ -59610,7 +59568,7 @@
     </row>
     <row r="1769" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1769" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1769" s="1" t="s">
         <v>3687</v>
@@ -59656,7 +59614,7 @@
     </row>
     <row r="1771" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1771" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1771" s="1" t="s">
         <v>3691</v>
@@ -59794,7 +59752,7 @@
     </row>
     <row r="1777" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1777" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B1777" s="1" t="s">
         <v>3703</v>
@@ -59932,7 +59890,7 @@
     </row>
     <row r="1783" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1783" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1783" s="1" t="s">
         <v>3718</v>
@@ -59955,7 +59913,7 @@
     </row>
     <row r="1784" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1784" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1784" s="1" t="s">
         <v>3719</v>
@@ -60231,7 +60189,7 @@
     </row>
     <row r="1796" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1796" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1796" s="1" t="s">
         <v>3739</v>
@@ -60553,7 +60511,7 @@
     </row>
     <row r="1810" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1810" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1810" s="1" t="s">
         <v>3757</v>
@@ -60576,7 +60534,7 @@
     </row>
     <row r="1811" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1811" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1811" s="1" t="s">
         <v>3758</v>
@@ -60645,7 +60603,7 @@
     </row>
     <row r="1814" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1814" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1814" s="1" t="s">
         <v>3761</v>
@@ -60691,7 +60649,7 @@
     </row>
     <row r="1816" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1816" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1816" s="1" t="s">
         <v>3765</v>
@@ -60852,7 +60810,7 @@
     </row>
     <row r="1823" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1823" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1823" s="1" t="s">
         <v>3775</v>
@@ -60898,7 +60856,7 @@
     </row>
     <row r="1825" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1825" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1825" s="1" t="s">
         <v>3781</v>
@@ -60921,7 +60879,7 @@
     </row>
     <row r="1826" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1826" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1826" s="1" t="s">
         <v>3784</v>
@@ -60944,7 +60902,7 @@
     </row>
     <row r="1827" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1827" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1827" s="1" t="s">
         <v>3786</v>
@@ -60990,7 +60948,7 @@
     </row>
     <row r="1829" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1829" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1829" s="1" t="s">
         <v>3792</v>
@@ -61013,7 +60971,7 @@
     </row>
     <row r="1830" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1830" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1830" s="1" t="s">
         <v>3795</v>
@@ -61082,7 +61040,7 @@
     </row>
     <row r="1833" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1833" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B1833" s="1" t="s">
         <v>3804</v>
@@ -61105,7 +61063,7 @@
     </row>
     <row r="1834" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1834" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1834" s="1" t="s">
         <v>3805</v>
@@ -61151,7 +61109,7 @@
     </row>
     <row r="1836" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1836" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1836" s="1" t="s">
         <v>3807</v>
@@ -61312,7 +61270,7 @@
     </row>
     <row r="1843" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1843" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1843" s="1" t="s">
         <v>3823</v>
@@ -61335,7 +61293,7 @@
     </row>
     <row r="1844" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1844" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1844" s="1" t="s">
         <v>3826</v>
@@ -61416,12 +61374,12 @@
         <v>3836</v>
       </c>
       <c r="G1847" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1848" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1848" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1848" s="1" t="s">
         <v>3837</v>
@@ -61467,7 +61425,7 @@
     </row>
     <row r="1850" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1850" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1850" s="1" t="s">
         <v>3841</v>
@@ -61697,7 +61655,7 @@
     </row>
     <row r="1860" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1860" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1860" s="1" t="s">
         <v>3860</v>
@@ -61720,7 +61678,7 @@
     </row>
     <row r="1861" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1861" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1861" s="1" t="s">
         <v>3863</v>
@@ -61801,12 +61759,12 @@
         <v>3872</v>
       </c>
       <c r="G1864" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1865" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1865" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1865" s="1" t="s">
         <v>3873</v>
@@ -61829,7 +61787,7 @@
     </row>
     <row r="1866" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1866" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1866" s="1" t="s">
         <v>3874</v>
@@ -62460,7 +62418,7 @@
         <v>62</v>
       </c>
       <c r="G1893" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1894" spans="1:7" x14ac:dyDescent="0.3">
@@ -63059,7 +63017,7 @@
     </row>
     <row r="1920" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1920" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B1920" s="1" t="s">
         <v>3985</v>
@@ -63105,7 +63063,7 @@
     </row>
     <row r="1922" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1922" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B1922" s="1" t="s">
         <v>3988</v>
@@ -63266,7 +63224,7 @@
     </row>
     <row r="1929" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1929" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1929" s="1" t="s">
         <v>4003</v>
@@ -63335,7 +63293,7 @@
     </row>
     <row r="1932" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1932" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1932" s="1" t="s">
         <v>4010</v>
@@ -63542,7 +63500,7 @@
     </row>
     <row r="1941" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1941" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1941" s="1" t="s">
         <v>4023</v>
@@ -63588,7 +63546,7 @@
     </row>
     <row r="1943" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1943" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1943" s="1" t="s">
         <v>4025</v>
@@ -63749,7 +63707,7 @@
     </row>
     <row r="1950" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1950" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1950" s="1" t="s">
         <v>4038</v>
@@ -64002,7 +63960,7 @@
     </row>
     <row r="1961" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1961" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1961" s="1" t="s">
         <v>4057</v>
@@ -64025,7 +63983,7 @@
     </row>
     <row r="1962" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1962" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1962" s="1" t="s">
         <v>4058</v>
@@ -64048,7 +64006,7 @@
     </row>
     <row r="1963" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1963" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1963" s="1" t="s">
         <v>4059</v>
@@ -64140,7 +64098,7 @@
     </row>
     <row r="1967" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1967" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B1967" s="1" t="s">
         <v>4065</v>
@@ -64186,7 +64144,7 @@
     </row>
     <row r="1969" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1969" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B1969" s="1" t="s">
         <v>4069</v>
@@ -64439,7 +64397,7 @@
     </row>
     <row r="1980" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1980" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1980" s="1" t="s">
         <v>4088</v>
@@ -64462,7 +64420,7 @@
     </row>
     <row r="1981" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1981" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B1981" s="1" t="s">
         <v>4089</v>
@@ -64587,7 +64545,7 @@
         <v>62</v>
       </c>
       <c r="G1986" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="1987" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -65029,7 +64987,7 @@
     </row>
     <row r="2006" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2006" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B2006" s="1" t="s">
         <v>4123</v>
@@ -65052,7 +65010,7 @@
     </row>
     <row r="2007" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2007" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B2007" s="1" t="s">
         <v>4126</v>
@@ -65098,7 +65056,7 @@
     </row>
     <row r="2009" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2009" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B2009" s="1" t="s">
         <v>4130</v>
@@ -65190,7 +65148,7 @@
     </row>
     <row r="2013" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2013" s="2" t="s">
-        <v>6049</v>
+        <v>3778</v>
       </c>
       <c r="B2013" s="1" t="s">
         <v>4136</v>
@@ -65282,7 +65240,7 @@
     </row>
     <row r="2017" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2017" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B2017" s="1" t="s">
         <v>4142</v>
@@ -65328,7 +65286,7 @@
     </row>
     <row r="2019" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2019" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B2019" s="1" t="s">
         <v>4144</v>
@@ -65558,7 +65516,7 @@
     </row>
     <row r="2029" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2029" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B2029" s="1" t="s">
         <v>4164</v>
@@ -65650,7 +65608,7 @@
     </row>
     <row r="2033" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2033" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B2033" s="1" t="s">
         <v>4170</v>
@@ -65673,7 +65631,7 @@
     </row>
     <row r="2034" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2034" s="2" t="s">
-        <v>6043</v>
+        <v>304</v>
       </c>
       <c r="B2034" s="1" t="s">
         <v>4172</v>
@@ -65725,7 +65683,7 @@
         <v>4176</v>
       </c>
       <c r="G2036" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2037" spans="1:7" x14ac:dyDescent="0.3">
@@ -65740,7 +65698,7 @@
         <v>62</v>
       </c>
       <c r="G2037" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2038" spans="1:7" x14ac:dyDescent="0.3">
@@ -65860,7 +65818,7 @@
     </row>
     <row r="2043" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2043" s="2" t="s">
-        <v>6047</v>
+        <v>2561</v>
       </c>
       <c r="B2043" s="1" t="s">
         <v>4187</v>
@@ -65975,7 +65933,7 @@
     </row>
     <row r="2048" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2048" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B2048" s="1" t="s">
         <v>4196</v>
@@ -66067,7 +66025,7 @@
     </row>
     <row r="2052" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2052" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B2052" s="1" t="s">
         <v>4204</v>
@@ -66320,7 +66278,7 @@
     </row>
     <row r="2063" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2063" s="2" t="s">
-        <v>6050</v>
+        <v>4228</v>
       </c>
       <c r="B2063" s="1" t="s">
         <v>4226</v>
@@ -66343,7 +66301,7 @@
     </row>
     <row r="2064" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2064" s="2" t="s">
-        <v>6050</v>
+        <v>4228</v>
       </c>
       <c r="B2064" s="1" t="s">
         <v>4229</v>
@@ -66481,7 +66439,7 @@
     </row>
     <row r="2070" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2070" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B2070" s="1" t="s">
         <v>4241</v>
@@ -67332,7 +67290,7 @@
     </row>
     <row r="2107" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2107" s="2" t="s">
-        <v>6050</v>
+        <v>4228</v>
       </c>
       <c r="B2107" s="1" t="s">
         <v>4300</v>
@@ -67424,7 +67382,7 @@
     </row>
     <row r="2111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2111" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2111" s="1" t="s">
         <v>4312</v>
@@ -67447,7 +67405,7 @@
     </row>
     <row r="2112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2112" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2112" s="1" t="s">
         <v>4313</v>
@@ -68965,7 +68923,7 @@
     </row>
     <row r="2178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2178" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B2178" s="1" t="s">
         <v>4405</v>
@@ -68988,7 +68946,7 @@
     </row>
     <row r="2179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2179" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B2179" s="1" t="s">
         <v>4407</v>
@@ -69034,7 +68992,7 @@
     </row>
     <row r="2181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2181" s="2" t="s">
-        <v>6046</v>
+        <v>1929</v>
       </c>
       <c r="B2181" s="1" t="s">
         <v>4412</v>
@@ -69126,7 +69084,7 @@
     </row>
     <row r="2185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2185" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B2185" s="1" t="s">
         <v>4419</v>
@@ -69161,12 +69119,12 @@
         <v>4423</v>
       </c>
       <c r="G2186" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2187" s="2" t="s">
-        <v>6045</v>
+        <v>920</v>
       </c>
       <c r="B2187" s="1" t="s">
         <v>4425</v>
@@ -69408,7 +69366,7 @@
         <v>4440</v>
       </c>
       <c r="G2197" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2198" spans="1:7" x14ac:dyDescent="0.3">
@@ -69676,7 +69634,7 @@
         <v>62</v>
       </c>
       <c r="G2209" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2210" spans="1:7" x14ac:dyDescent="0.3">
@@ -69691,7 +69649,7 @@
         <v>62</v>
       </c>
       <c r="G2210" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2211" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -69823,7 +69781,7 @@
         <v>4467</v>
       </c>
       <c r="G2216" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2217" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -69884,7 +69842,7 @@
         <v>62</v>
       </c>
       <c r="G2219" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2220" spans="1:7" x14ac:dyDescent="0.3">
@@ -70014,7 +69972,7 @@
         <v>640</v>
       </c>
       <c r="G2225" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2226" spans="1:7" x14ac:dyDescent="0.3">
@@ -70397,7 +70355,7 @@
         <v>62</v>
       </c>
       <c r="G2242" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2243" spans="1:7" x14ac:dyDescent="0.3">
@@ -70713,7 +70671,7 @@
         <v>4539</v>
       </c>
       <c r="G2256" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2257" spans="1:7" x14ac:dyDescent="0.3">
@@ -70797,7 +70755,7 @@
         <v>640</v>
       </c>
       <c r="G2260" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2261" spans="1:7" x14ac:dyDescent="0.3">
@@ -72263,7 +72221,7 @@
         <v>4678</v>
       </c>
       <c r="G2324" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2325" spans="1:7" x14ac:dyDescent="0.3">
@@ -73648,7 +73606,7 @@
         <v>4789</v>
       </c>
       <c r="G2385" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2386" spans="1:7" x14ac:dyDescent="0.3">
@@ -73895,7 +73853,7 @@
         <v>4811</v>
       </c>
       <c r="G2396" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2397" spans="1:7" x14ac:dyDescent="0.3">
@@ -74107,7 +74065,7 @@
     </row>
     <row r="2406" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2406" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2406" s="1" t="s">
         <v>4829</v>
@@ -74153,7 +74111,7 @@
     </row>
     <row r="2408" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2408" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2408" s="1" t="s">
         <v>4833</v>
@@ -74498,7 +74456,7 @@
     </row>
     <row r="2423" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2423" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2423" s="1" t="s">
         <v>4874</v>
@@ -75671,7 +75629,7 @@
     </row>
     <row r="2474" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2474" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2474" s="1" t="s">
         <v>4948</v>
@@ -75786,7 +75744,7 @@
     </row>
     <row r="2479" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2479" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2479" s="1" t="s">
         <v>4960</v>
@@ -75924,7 +75882,7 @@
     </row>
     <row r="2485" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2485" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2485" s="1" t="s">
         <v>4974</v>
@@ -76177,7 +76135,7 @@
     </row>
     <row r="2496" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2496" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2496" s="1" t="s">
         <v>4996</v>
@@ -76269,7 +76227,7 @@
     </row>
     <row r="2500" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2500" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2500" s="1" t="s">
         <v>5001</v>
@@ -76292,7 +76250,7 @@
     </row>
     <row r="2501" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2501" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2501" s="1" t="s">
         <v>5003</v>
@@ -76338,7 +76296,7 @@
     </row>
     <row r="2503" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2503" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2503" s="1" t="s">
         <v>5007</v>
@@ -76384,7 +76342,7 @@
     </row>
     <row r="2505" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2505" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2505" s="1" t="s">
         <v>5011</v>
@@ -76407,7 +76365,7 @@
     </row>
     <row r="2506" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2506" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2506" s="1" t="s">
         <v>5012</v>
@@ -76798,7 +76756,7 @@
     </row>
     <row r="2523" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2523" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2523" s="1" t="s">
         <v>5046</v>
@@ -76844,7 +76802,7 @@
     </row>
     <row r="2525" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2525" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2525" s="1" t="s">
         <v>5051</v>
@@ -76936,7 +76894,7 @@
     </row>
     <row r="2529" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2529" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2529" s="1" t="s">
         <v>5061</v>
@@ -76959,7 +76917,7 @@
     </row>
     <row r="2530" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2530" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2530" s="1" t="s">
         <v>5064</v>
@@ -77005,7 +76963,7 @@
     </row>
     <row r="2532" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2532" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2532" s="1" t="s">
         <v>5070</v>
@@ -77028,7 +76986,7 @@
     </row>
     <row r="2533" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2533" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2533" s="1" t="s">
         <v>5073</v>
@@ -77061,12 +77019,12 @@
         <v>62</v>
       </c>
       <c r="G2534" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2535" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2535" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2535" s="1" t="s">
         <v>5076</v>
@@ -77099,7 +77057,7 @@
         <v>62</v>
       </c>
       <c r="G2536" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2537" spans="1:7" x14ac:dyDescent="0.3">
@@ -77114,7 +77072,7 @@
         <v>62</v>
       </c>
       <c r="G2537" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2538" spans="1:7" x14ac:dyDescent="0.3">
@@ -77129,7 +77087,7 @@
         <v>62</v>
       </c>
       <c r="G2538" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2539" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -77190,7 +77148,7 @@
         <v>62</v>
       </c>
       <c r="G2541" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2542" spans="1:7" x14ac:dyDescent="0.3">
@@ -77205,7 +77163,7 @@
         <v>62</v>
       </c>
       <c r="G2542" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2543" spans="1:7" x14ac:dyDescent="0.3">
@@ -77279,7 +77237,7 @@
     </row>
     <row r="2546" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2546" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2546" s="1" t="s">
         <v>5095</v>
@@ -77532,7 +77490,7 @@
     </row>
     <row r="2557" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2557" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2557" s="1" t="s">
         <v>5118</v>
@@ -77601,7 +77559,7 @@
     </row>
     <row r="2560" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2560" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2560" s="1" t="s">
         <v>5125</v>
@@ -77762,7 +77720,7 @@
     </row>
     <row r="2567" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2567" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2567" s="1" t="s">
         <v>5140</v>
@@ -77795,12 +77753,12 @@
         <v>62</v>
       </c>
       <c r="G2568" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2569" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2569" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2569" s="1" t="s">
         <v>5144</v>
@@ -77846,7 +77804,7 @@
     </row>
     <row r="2571" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2571" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2571" s="1" t="s">
         <v>5147</v>
@@ -77915,7 +77873,7 @@
     </row>
     <row r="2574" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2574" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2574" s="1" t="s">
         <v>5154</v>
@@ -78053,7 +78011,7 @@
     </row>
     <row r="2580" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2580" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2580" s="1" t="s">
         <v>5170</v>
@@ -78237,7 +78195,7 @@
     </row>
     <row r="2588" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2588" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2588" s="1" t="s">
         <v>5188</v>
@@ -78270,7 +78228,7 @@
         <v>62</v>
       </c>
       <c r="G2589" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2590" spans="1:7" x14ac:dyDescent="0.3">
@@ -78954,7 +78912,7 @@
         <v>5252</v>
       </c>
       <c r="G2619" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2620" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -79419,7 +79377,7 @@
     </row>
     <row r="2640" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2640" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2640" s="1" t="s">
         <v>5293</v>
@@ -79810,7 +79768,7 @@
     </row>
     <row r="2657" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2657" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2657" s="1" t="s">
         <v>5333</v>
@@ -80063,7 +80021,7 @@
     </row>
     <row r="2668" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2668" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2668" s="1" t="s">
         <v>5357</v>
@@ -80339,7 +80297,7 @@
     </row>
     <row r="2680" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2680" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2680" s="1" t="s">
         <v>5389</v>
@@ -80592,7 +80550,7 @@
     </row>
     <row r="2691" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2691" s="2" t="s">
-        <v>6042</v>
+        <v>180</v>
       </c>
       <c r="B2691" s="1" t="s">
         <v>5414</v>
@@ -80799,7 +80757,7 @@
     </row>
     <row r="2700" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2700" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2700" s="1" t="s">
         <v>5434</v>
@@ -81374,7 +81332,7 @@
     </row>
     <row r="2725" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2725" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2725" s="1" t="s">
         <v>5483</v>
@@ -81466,7 +81424,7 @@
     </row>
     <row r="2729" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2729" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2729" s="1" t="s">
         <v>5488</v>
@@ -81489,7 +81447,7 @@
     </row>
     <row r="2730" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2730" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2730" s="1" t="s">
         <v>5491</v>
@@ -81696,7 +81654,7 @@
     </row>
     <row r="2739" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2739" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2739" s="1" t="s">
         <v>5507</v>
@@ -81765,7 +81723,7 @@
     </row>
     <row r="2742" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2742" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2742" s="1" t="s">
         <v>5512</v>
@@ -81811,7 +81769,7 @@
     </row>
     <row r="2744" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2744" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2744" s="1" t="s">
         <v>5514</v>
@@ -82179,7 +82137,7 @@
     </row>
     <row r="2760" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2760" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2760" s="1" t="s">
         <v>5539</v>
@@ -82271,7 +82229,7 @@
     </row>
     <row r="2764" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2764" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2764" s="1" t="s">
         <v>5543</v>
@@ -82639,7 +82597,7 @@
     </row>
     <row r="2780" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2780" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B2780" s="1" t="s">
         <v>5583</v>
@@ -82915,7 +82873,7 @@
     </row>
     <row r="2792" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2792" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2792" s="1" t="s">
         <v>5610</v>
@@ -83099,7 +83057,7 @@
     </row>
     <row r="2800" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2800" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2800" s="1" t="s">
         <v>5628</v>
@@ -83168,7 +83126,7 @@
     </row>
     <row r="2803" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2803" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2803" s="1" t="s">
         <v>5631</v>
@@ -83455,7 +83413,7 @@
     </row>
     <row r="2816" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2816" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B2816" s="1" t="s">
         <v>5658</v>
@@ -83605,7 +83563,7 @@
         <v>5671</v>
       </c>
       <c r="G2822" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2823" spans="1:7" x14ac:dyDescent="0.3">
@@ -83873,7 +83831,7 @@
         <v>62</v>
       </c>
       <c r="G2834" t="s">
-        <v>6051</v>
+        <v>6037</v>
       </c>
     </row>
     <row r="2835" spans="1:7" x14ac:dyDescent="0.3">
@@ -85273,7 +85231,7 @@
     </row>
     <row r="2896" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2896" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B2896" s="1" t="s">
         <v>5806</v>
@@ -85480,7 +85438,7 @@
     </row>
     <row r="2905" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2905" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2905" s="1" t="s">
         <v>5825</v>
@@ -85503,7 +85461,7 @@
     </row>
     <row r="2906" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2906" s="2" t="s">
-        <v>6041</v>
+        <v>166</v>
       </c>
       <c r="B2906" s="1" t="s">
         <v>5827</v>
@@ -85660,7 +85618,7 @@
     </row>
     <row r="2913" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2913" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2913" s="1" t="s">
         <v>5842</v>
@@ -85821,7 +85779,7 @@
     </row>
     <row r="2920" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2920" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2920" s="1" t="s">
         <v>5853</v>
@@ -85844,7 +85802,7 @@
     </row>
     <row r="2921" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2921" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2921" s="1" t="s">
         <v>5855</v>
@@ -85867,7 +85825,7 @@
     </row>
     <row r="2922" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2922" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2922" s="1" t="s">
         <v>5856</v>
@@ -85955,7 +85913,7 @@
     </row>
     <row r="2926" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2926" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2926" s="1" t="s">
         <v>5866</v>
@@ -86185,7 +86143,7 @@
     </row>
     <row r="2936" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2936" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2936" s="1" t="s">
         <v>5886</v>
@@ -86208,7 +86166,7 @@
     </row>
     <row r="2937" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2937" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2937" s="1" t="s">
         <v>5887</v>
@@ -86231,7 +86189,7 @@
     </row>
     <row r="2938" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2938" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2938" s="1" t="s">
         <v>5890</v>
@@ -86392,7 +86350,7 @@
     </row>
     <row r="2945" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2945" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2945" s="1" t="s">
         <v>5907</v>
@@ -86438,7 +86396,7 @@
     </row>
     <row r="2947" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2947" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2947" s="1" t="s">
         <v>5909</v>
@@ -86622,7 +86580,7 @@
     </row>
     <row r="2955" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2955" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2955" s="1" t="s">
         <v>5927</v>
@@ -86645,7 +86603,7 @@
     </row>
     <row r="2956" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2956" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2956" s="1" t="s">
         <v>5929</v>
@@ -86760,7 +86718,7 @@
     </row>
     <row r="2961" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2961" s="2" t="s">
-        <v>6039</v>
+        <v>99</v>
       </c>
       <c r="B2961" s="1" t="s">
         <v>5940</v>
@@ -87534,7 +87492,7 @@
     </row>
     <row r="2995" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2995" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2995" s="1" t="s">
         <v>6007</v>
@@ -87557,7 +87515,7 @@
     </row>
     <row r="2996" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2996" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2996" s="1" t="s">
         <v>6008</v>
@@ -87580,7 +87538,7 @@
     </row>
     <row r="2997" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2997" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2997" s="1" t="s">
         <v>6009</v>
@@ -87603,7 +87561,7 @@
     </row>
     <row r="2998" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2998" s="2" t="s">
-        <v>6038</v>
+        <v>45</v>
       </c>
       <c r="B2998" s="1" t="s">
         <v>6011</v>
@@ -87741,7 +87699,7 @@
     </row>
     <row r="3004" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3004" s="2" t="s">
-        <v>6037</v>
+        <v>16</v>
       </c>
       <c r="B3004" s="1" t="s">
         <v>6021</v>
@@ -87902,7 +87860,7 @@
     </row>
     <row r="3011" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3011" s="2" t="s">
-        <v>6044</v>
+        <v>402</v>
       </c>
       <c r="B3011" s="1" t="s">
         <v>6032</v>

</xml_diff>